<commit_message>
Form build from JSON working
</commit_message>
<xml_diff>
--- a/Readme.xlsx
+++ b/Readme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif\OneDrive\My_Projects\Mine\Apps\MedicalFormsApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asif\OneDrive\My_Projects\Mine\Apps\Forms - Medical App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B163EB-2385-42E2-8593-7743D0142323}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB894B0-529D-486E-89F1-6C1E7CC038C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>No.</t>
   </si>
@@ -88,6 +88,27 @@
   <si>
     <t>Git folder tracking changes and commits. Source files are hosted on GitHub in a Private Repo.</t>
   </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>certificate.crt</t>
+  </si>
+  <si>
+    <t>privateKey.key</t>
+  </si>
+  <si>
+    <t>Required for testing voicerecognition on mobile browser. Without it cannot get access to the microphone. Also used in live server (in visual studio code). Companion file is certificate.crt</t>
+  </si>
+  <si>
+    <t>C:\Users\Asif\OneDrive\My_Projects\Mine\Apps\Forms - Medical App\Certificates</t>
+  </si>
+  <si>
+    <t>Required for testing voicerecognition on mobile browser. Without it cannot get access to the microphone. Also used in live server (in visual studio code). Companion file is privateKey.key
+Had to install Openssl
+Command: req -x509 -sha256 -nodes -days 365 -newkey rsa:2048 -keyout privateKey.key -out certificate.crt
+Run as administrator otherwise wont save the files</t>
+  </si>
 </sst>
 </file>
 
@@ -122,8 +143,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14858,14 +14882,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41AF5033-F417-4FC3-B7C6-77CD51345174}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0">
-  <autoFilter ref="A1:D9" xr:uid="{3B7235C3-6908-4157-8EF9-C5244C6B6B9B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41AF5033-F417-4FC3-B7C6-77CD51345174}" name="Table1" displayName="Table1" ref="A1:E10" totalsRowShown="0">
+  <autoFilter ref="A1:E10" xr:uid="{3B7235C3-6908-4157-8EF9-C5244C6B6B9B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
     <sortCondition ref="A1:A9"/>
   </sortState>
-  <tableColumns count="4">
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{ACCC6779-1758-4157-9E5F-33A726478E11}" name="No."/>
     <tableColumn id="2" xr3:uid="{2268FAEC-7595-47B2-9770-396C7DFE7E61}" name="File/Folder Name"/>
+    <tableColumn id="4" xr3:uid="{7D7FB618-E521-4A4A-982B-9C5561678805}" name="Location"/>
     <tableColumn id="5" xr3:uid="{FE1B1D29-1EB5-4D3A-8934-011AF68E3828}" name="File or Folder"/>
     <tableColumn id="3" xr3:uid="{A75A6A09-A7A0-4131-939D-E93AC59A4B65}" name="Purpose"/>
   </tableColumns>
@@ -15136,21 +15161,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="122" customWidth="1"/>
+    <col min="2" max="3" width="26.77734375" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="98.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -15158,117 +15183,149 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Folder"</formula>
     </cfRule>
@@ -15277,7 +15334,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{F4F7E71D-B77E-4D4D-8FA6-9329D67649A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{F4F7E71D-B77E-4D4D-8FA6-9329D67649A5}">
       <formula1>"File, Folder"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15308,7 +15365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F781D020-8667-4CA7-BAA1-16B72F335F84}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>

</xml_diff>